<commit_message>
add second strategy chart
</commit_message>
<xml_diff>
--- a/data/strategy_charts.xlsx
+++ b/data/strategy_charts.xlsx
@@ -4,6 +4,7 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Chart1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Chart2" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="24">
   <si>
     <t>A</t>
   </si>
@@ -132,6 +133,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -1564,4 +1569,1241 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="C1" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="D1" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="E1" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="F1" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="G1" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="H1" s="1">
+        <v>8.0</v>
+      </c>
+      <c r="I1" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="J1" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1">
+        <v>8.0</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1">
+        <v>12.0</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1">
+        <v>13.0</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1">
+        <v>14.0</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1">
+        <v>15.0</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1">
+        <v>16.0</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1">
+        <v>17.0</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1">
+        <v>18.0</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1">
+        <v>19.0</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1">
+        <v>20.0</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add 4 to player hands
</commit_message>
<xml_diff>
--- a/data/strategy_charts.xlsx
+++ b/data/strategy_charts.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="24">
   <si>
     <t>A</t>
   </si>
@@ -383,7 +383,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
@@ -418,7 +418,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
@@ -453,7 +453,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>1</v>
@@ -488,7 +488,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1">
-        <v>8.0</v>
+        <v>7.0</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>1</v>
@@ -523,22 +523,22 @@
     </row>
     <row r="6">
       <c r="A6" s="1">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>1</v>
@@ -558,10 +558,10 @@
     </row>
     <row r="7">
       <c r="A7" s="1">
-        <v>10.0</v>
+        <v>9.0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>2</v>
@@ -576,13 +576,13 @@
         <v>2</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>1</v>
@@ -593,7 +593,7 @@
     </row>
     <row r="8">
       <c r="A8" s="1">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>2</v>
@@ -620,7 +620,7 @@
         <v>2</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>1</v>
@@ -628,34 +628,34 @@
     </row>
     <row r="9">
       <c r="A9" s="1">
-        <v>12.0</v>
+        <v>11.0</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>1</v>
@@ -663,13 +663,13 @@
     </row>
     <row r="10">
       <c r="A10" s="1">
-        <v>13.0</v>
+        <v>12.0</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>3</v>
@@ -698,7 +698,7 @@
     </row>
     <row r="11">
       <c r="A11" s="1">
-        <v>14.0</v>
+        <v>13.0</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>3</v>
@@ -733,7 +733,7 @@
     </row>
     <row r="12">
       <c r="A12" s="1">
-        <v>15.0</v>
+        <v>14.0</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>3</v>
@@ -760,7 +760,7 @@
         <v>1</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>1</v>
@@ -768,7 +768,7 @@
     </row>
     <row r="13">
       <c r="A13" s="1">
-        <v>16.0</v>
+        <v>15.0</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>3</v>
@@ -792,18 +792,18 @@
         <v>1</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1">
-        <v>17.0</v>
+        <v>16.0</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>3</v>
@@ -821,24 +821,24 @@
         <v>3</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1">
-        <v>18.0</v>
+        <v>17.0</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>3</v>
@@ -873,7 +873,7 @@
     </row>
     <row r="16">
       <c r="A16" s="1">
-        <v>19.0</v>
+        <v>18.0</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>3</v>
@@ -908,77 +908,77 @@
     </row>
     <row r="17">
       <c r="A17" s="1">
+        <v>19.0</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1">
         <v>20.0</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="B18" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>1</v>
@@ -1013,7 +1013,7 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>1</v>
@@ -1022,7 +1022,7 @@
         <v>1</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>2</v>
@@ -1048,7 +1048,7 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>1</v>
@@ -1083,13 +1083,13 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>2</v>
@@ -1118,10 +1118,10 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>2</v>
@@ -1136,10 +1136,10 @@
         <v>2</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>1</v>
@@ -1153,22 +1153,22 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>3</v>
@@ -1177,18 +1177,18 @@
         <v>3</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>3</v>
@@ -1223,42 +1223,42 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>14</v>
@@ -1293,16 +1293,16 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>14</v>
@@ -1311,7 +1311,7 @@
         <v>14</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>1</v>
@@ -1328,31 +1328,31 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>1</v>
@@ -1363,31 +1363,31 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>1</v>
@@ -1398,7 +1398,7 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>14</v>
@@ -1416,7 +1416,7 @@
         <v>14</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>1</v>
@@ -1433,7 +1433,7 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>14</v>
@@ -1454,21 +1454,21 @@
         <v>14</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>14</v>
@@ -1486,7 +1486,7 @@
         <v>14</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>14</v>
@@ -1495,39 +1495,39 @@
         <v>14</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>3</v>
@@ -1538,36 +1538,71 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I35" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J35" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K35" s="1" t="s">
+      <c r="B36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K36" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1620,7 +1655,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
@@ -1655,7 +1690,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
@@ -1690,7 +1725,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>1</v>
@@ -1725,7 +1760,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1">
-        <v>8.0</v>
+        <v>7.0</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>1</v>
@@ -1760,22 +1795,22 @@
     </row>
     <row r="6">
       <c r="A6" s="1">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>1</v>
@@ -1795,10 +1830,10 @@
     </row>
     <row r="7">
       <c r="A7" s="1">
-        <v>10.0</v>
+        <v>9.0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>2</v>
@@ -1813,13 +1848,13 @@
         <v>2</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>1</v>
@@ -1830,7 +1865,7 @@
     </row>
     <row r="8">
       <c r="A8" s="1">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>2</v>
@@ -1857,7 +1892,7 @@
         <v>2</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>1</v>
@@ -1865,34 +1900,34 @@
     </row>
     <row r="9">
       <c r="A9" s="1">
-        <v>12.0</v>
+        <v>11.0</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>1</v>
@@ -1900,13 +1935,13 @@
     </row>
     <row r="10">
       <c r="A10" s="1">
-        <v>13.0</v>
+        <v>12.0</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>3</v>
@@ -1935,7 +1970,7 @@
     </row>
     <row r="11">
       <c r="A11" s="1">
-        <v>14.0</v>
+        <v>13.0</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>3</v>
@@ -1970,7 +2005,7 @@
     </row>
     <row r="12">
       <c r="A12" s="1">
-        <v>15.0</v>
+        <v>14.0</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>3</v>
@@ -2005,7 +2040,7 @@
     </row>
     <row r="13">
       <c r="A13" s="1">
-        <v>16.0</v>
+        <v>15.0</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>3</v>
@@ -2040,7 +2075,7 @@
     </row>
     <row r="14">
       <c r="A14" s="1">
-        <v>17.0</v>
+        <v>16.0</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>3</v>
@@ -2058,24 +2093,24 @@
         <v>3</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1">
-        <v>18.0</v>
+        <v>17.0</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>3</v>
@@ -2110,7 +2145,7 @@
     </row>
     <row r="16">
       <c r="A16" s="1">
-        <v>19.0</v>
+        <v>18.0</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>3</v>
@@ -2145,77 +2180,77 @@
     </row>
     <row r="17">
       <c r="A17" s="1">
+        <v>19.0</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1">
         <v>20.0</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="B18" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>1</v>
@@ -2250,7 +2285,7 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>1</v>
@@ -2259,7 +2294,7 @@
         <v>1</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>2</v>
@@ -2285,7 +2320,7 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>1</v>
@@ -2320,13 +2355,13 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>2</v>
@@ -2355,10 +2390,10 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>2</v>
@@ -2373,10 +2408,10 @@
         <v>2</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>1</v>
@@ -2390,22 +2425,22 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>3</v>
@@ -2414,18 +2449,18 @@
         <v>3</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>3</v>
@@ -2460,42 +2495,42 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>14</v>
@@ -2530,16 +2565,16 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>14</v>
@@ -2548,7 +2583,7 @@
         <v>14</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>1</v>
@@ -2565,31 +2600,31 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>1</v>
@@ -2600,31 +2635,31 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>1</v>
@@ -2635,7 +2670,7 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>14</v>
@@ -2653,7 +2688,7 @@
         <v>14</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>1</v>
@@ -2670,7 +2705,7 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>14</v>
@@ -2691,21 +2726,21 @@
         <v>14</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>14</v>
@@ -2723,7 +2758,7 @@
         <v>14</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>14</v>
@@ -2732,39 +2767,39 @@
         <v>14</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>3</v>
@@ -2775,36 +2810,71 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I35" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J35" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K35" s="1" t="s">
+      <c r="B36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K36" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2857,7 +2927,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
@@ -2892,7 +2962,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
@@ -2927,7 +2997,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>1</v>
@@ -2962,7 +3032,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1">
-        <v>8.0</v>
+        <v>7.0</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>1</v>
@@ -2997,22 +3067,22 @@
     </row>
     <row r="6">
       <c r="A6" s="1">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>1</v>
@@ -3032,10 +3102,10 @@
     </row>
     <row r="7">
       <c r="A7" s="1">
-        <v>10.0</v>
+        <v>9.0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>2</v>
@@ -3050,13 +3120,13 @@
         <v>2</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>1</v>
@@ -3067,7 +3137,7 @@
     </row>
     <row r="8">
       <c r="A8" s="1">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>2</v>
@@ -3094,7 +3164,7 @@
         <v>2</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>1</v>
@@ -3102,34 +3172,34 @@
     </row>
     <row r="9">
       <c r="A9" s="1">
-        <v>12.0</v>
+        <v>11.0</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>1</v>
@@ -3137,13 +3207,13 @@
     </row>
     <row r="10">
       <c r="A10" s="1">
-        <v>13.0</v>
+        <v>12.0</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>3</v>
@@ -3172,7 +3242,7 @@
     </row>
     <row r="11">
       <c r="A11" s="1">
-        <v>14.0</v>
+        <v>13.0</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>3</v>
@@ -3207,7 +3277,7 @@
     </row>
     <row r="12">
       <c r="A12" s="1">
-        <v>15.0</v>
+        <v>14.0</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>3</v>
@@ -3234,7 +3304,7 @@
         <v>1</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>1</v>
@@ -3242,7 +3312,7 @@
     </row>
     <row r="13">
       <c r="A13" s="1">
-        <v>16.0</v>
+        <v>15.0</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>3</v>
@@ -3266,18 +3336,18 @@
         <v>1</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>3</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1">
-        <v>17.0</v>
+        <v>16.0</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>3</v>
@@ -3295,10 +3365,10 @@
         <v>3</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>3</v>
@@ -3312,7 +3382,7 @@
     </row>
     <row r="15">
       <c r="A15" s="1">
-        <v>18.0</v>
+        <v>17.0</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>3</v>
@@ -3347,7 +3417,7 @@
     </row>
     <row r="16">
       <c r="A16" s="1">
-        <v>19.0</v>
+        <v>18.0</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>3</v>
@@ -3382,77 +3452,77 @@
     </row>
     <row r="17">
       <c r="A17" s="1">
+        <v>19.0</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1">
         <v>20.0</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="B18" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>1</v>
@@ -3487,7 +3557,7 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>1</v>
@@ -3496,7 +3566,7 @@
         <v>1</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>2</v>
@@ -3522,7 +3592,7 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>1</v>
@@ -3557,13 +3627,13 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>2</v>
@@ -3592,10 +3662,10 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>2</v>
@@ -3610,10 +3680,10 @@
         <v>2</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>1</v>
@@ -3627,22 +3697,22 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>3</v>
@@ -3651,18 +3721,18 @@
         <v>3</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>3</v>
@@ -3697,42 +3767,42 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>14</v>
@@ -3767,16 +3837,16 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>14</v>
@@ -3785,7 +3855,7 @@
         <v>14</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>1</v>
@@ -3802,31 +3872,31 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>1</v>
@@ -3837,31 +3907,31 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>1</v>
@@ -3872,7 +3942,7 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>14</v>
@@ -3890,7 +3960,7 @@
         <v>14</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>1</v>
@@ -3907,7 +3977,7 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>14</v>
@@ -3928,21 +3998,21 @@
         <v>14</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>14</v>
@@ -3960,7 +4030,7 @@
         <v>14</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>14</v>
@@ -3969,39 +4039,39 @@
         <v>14</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>3</v>
@@ -4012,36 +4082,71 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I35" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J35" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K35" s="1" t="s">
+      <c r="B36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K36" s="1" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>